<commit_message>
lots of functionality added, including the ability to parse documents
</commit_message>
<xml_diff>
--- a/inputs/NG_Meduim_and_Support_AAT.xlsx
+++ b/inputs/NG_Meduim_and_Support_AAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orla.delaney\Documents\Code\python_scripts\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE4B893-8476-4805-8B7F-B348843C8474}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F88504-18DC-4CC7-A35D-25C935FF0655}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technique" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="302">
   <si>
     <t>Column 1</t>
   </si>
@@ -929,6 +929,18 @@
   </si>
   <si>
     <t>Drying Oil</t>
+  </si>
+  <si>
+    <t>Poplar Panel</t>
+  </si>
+  <si>
+    <t>Wooden Panel</t>
+  </si>
+  <si>
+    <t>Yew Panel</t>
+  </si>
+  <si>
+    <t>Canvas%2C Transferred from Wood</t>
   </si>
 </sst>
 </file>
@@ -1843,7 +1855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2439,7 +2451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
@@ -2876,7 +2888,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2921,7 +2935,7 @@
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>301</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>189</v>
@@ -3185,7 +3199,7 @@
     </row>
     <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>240</v>
+        <v>298</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>241</v>
@@ -3358,7 +3372,7 @@
     </row>
     <row r="44" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>279</v>
@@ -3380,7 +3394,7 @@
     </row>
     <row r="46" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>284</v>
+        <v>300</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>285</v>

</xml_diff>

<commit_message>
large update towards final version
</commit_message>
<xml_diff>
--- a/inputs/NG_Meduim_and_Support_AAT.xlsx
+++ b/inputs/NG_Meduim_and_Support_AAT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orla.delaney\Documents\Code\python_scripts\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F88504-18DC-4CC7-A35D-25C935FF0655}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3376D44B-1378-4BA0-90C1-9438D0516420}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technique" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,14 @@
     <sheet name="Support Materials" sheetId="4" r:id="rId4"/>
     <sheet name="Support Type" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="324">
   <si>
     <t>Column 1</t>
   </si>
@@ -292,9 +294,6 @@
     <t>aat:300011727</t>
   </si>
   <si>
-    <t>chalk</t>
-  </si>
-  <si>
     <t>aat:300130920</t>
   </si>
   <si>
@@ -304,9 +303,6 @@
     <t>aat:300167812</t>
   </si>
   <si>
-    <t>wax crayons</t>
-  </si>
-  <si>
     <t>aat:300022415</t>
   </si>
   <si>
@@ -316,21 +312,12 @@
     <t>aat:300070114</t>
   </si>
   <si>
-    <t>gouache (paint)</t>
-  </si>
-  <si>
     <t>aat:300010957</t>
   </si>
   <si>
-    <t>bronze (metal)</t>
-  </si>
-  <si>
     <t>aat:300012862</t>
   </si>
   <si>
-    <t>charcoal (material)</t>
-  </si>
-  <si>
     <t>aat:300022440</t>
   </si>
   <si>
@@ -355,9 +342,6 @@
     <t>aat:300183750</t>
   </si>
   <si>
-    <t>encaustic paint</t>
-  </si>
-  <si>
     <t>aat:300014922</t>
   </si>
   <si>
@@ -376,15 +360,9 @@
     <t>aat:300015312</t>
   </si>
   <si>
-    <t>size (material)</t>
-  </si>
-  <si>
     <t>aat:300264831</t>
   </si>
   <si>
-    <t>gold leaf</t>
-  </si>
-  <si>
     <t>aat:300311191</t>
   </si>
   <si>
@@ -394,9 +372,6 @@
     <t>aat:300011051</t>
   </si>
   <si>
-    <t>wash (material)</t>
-  </si>
-  <si>
     <t>aat:300130811</t>
   </si>
   <si>
@@ -406,9 +381,6 @@
     <t>aat:300012940</t>
   </si>
   <si>
-    <t>gum resin</t>
-  </si>
-  <si>
     <t>aat:300012866</t>
   </si>
   <si>
@@ -421,30 +393,18 @@
     <t>aat:300011232</t>
   </si>
   <si>
-    <t>porphyry</t>
-  </si>
-  <si>
     <t>aat:300014292</t>
   </si>
   <si>
     <t>aat:300010676</t>
   </si>
   <si>
-    <t>tile (material)</t>
-  </si>
-  <si>
     <t>aat:300015050</t>
   </si>
   <si>
-    <t>oil paint (paint)</t>
-  </si>
-  <si>
     <t>aat:300122621</t>
   </si>
   <si>
-    <t>pastels (crayons)</t>
-  </si>
-  <si>
     <t>aat:300230810</t>
   </si>
   <si>
@@ -454,15 +414,9 @@
     <t>aat:300022452</t>
   </si>
   <si>
-    <t>pens (drawing and writing)</t>
-  </si>
-  <si>
     <t>aat:300011098</t>
   </si>
   <si>
-    <t>graphite (mineral)</t>
-  </si>
-  <si>
     <t>aat:300022443</t>
   </si>
   <si>
@@ -472,9 +426,6 @@
     <t>aat:300014927</t>
   </si>
   <si>
-    <t>plaster of Paris</t>
-  </si>
-  <si>
     <t>aat:300014925</t>
   </si>
   <si>
@@ -484,18 +435,12 @@
     <t>aat:300265199</t>
   </si>
   <si>
-    <t>silver leaf</t>
-  </si>
-  <si>
     <t>aat:300015062</t>
   </si>
   <si>
     <t>aat:300183742</t>
   </si>
   <si>
-    <t>egg-oil tempera</t>
-  </si>
-  <si>
     <t>skos:altLabel</t>
   </si>
   <si>
@@ -508,15 +453,9 @@
     <t>aat:300015045</t>
   </si>
   <si>
-    <t>watercolor (paint)</t>
-  </si>
-  <si>
     <t>aat:300011576</t>
   </si>
   <si>
-    <t>Carrara marble</t>
-  </si>
-  <si>
     <t>aat:300129784</t>
   </si>
   <si>
@@ -529,39 +468,21 @@
     <t>aat:300033973</t>
   </si>
   <si>
-    <t>drawings (visual works)</t>
-  </si>
-  <si>
     <t>aat:300078928</t>
   </si>
   <si>
-    <t>gouaches (paintings)</t>
-  </si>
-  <si>
     <t>aat:300181922</t>
   </si>
   <si>
-    <t>encaustic paintings (visual works)</t>
-  </si>
-  <si>
     <t>aat:300177433</t>
   </si>
   <si>
-    <t>frescoes (paintings)</t>
-  </si>
-  <si>
     <t>aat:300078925</t>
   </si>
   <si>
-    <t>watercolors (paintings)</t>
-  </si>
-  <si>
     <t>aat:300181918</t>
   </si>
   <si>
-    <t>acrylic paintings (visual works)</t>
-  </si>
-  <si>
     <t>aat:300033799</t>
   </si>
   <si>
@@ -571,9 +492,6 @@
     <t>aat:300015342</t>
   </si>
   <si>
-    <t>mosaics (visual works)</t>
-  </si>
-  <si>
     <t>NG Field</t>
   </si>
   <si>
@@ -589,27 +507,18 @@
     <t>aat:300011948</t>
   </si>
   <si>
-    <t>beech (wood)</t>
-  </si>
-  <si>
     <t>board</t>
   </si>
   <si>
     <t>aat:300014198</t>
   </si>
   <si>
-    <t>fiberboard</t>
-  </si>
-  <si>
     <t>canvas</t>
   </si>
   <si>
     <t>aat:300014078</t>
   </si>
   <si>
-    <t>canvas (textile material)</t>
-  </si>
-  <si>
     <t>canvas scrim</t>
   </si>
   <si>
@@ -640,36 +549,24 @@
     <t>aat:300012558</t>
   </si>
   <si>
-    <t>fir (wood)</t>
-  </si>
-  <si>
     <t>ivory</t>
   </si>
   <si>
     <t>aat:300011857</t>
   </si>
   <si>
-    <t>ivory (material)</t>
-  </si>
-  <si>
     <t>laminated board</t>
   </si>
   <si>
     <t>aat:300387449</t>
   </si>
   <si>
-    <t>laminated paper</t>
-  </si>
-  <si>
     <t>lime</t>
   </si>
   <si>
     <t>aat:300012457</t>
   </si>
   <si>
-    <t>common lime (wood)</t>
-  </si>
-  <si>
     <t>limewood</t>
   </si>
   <si>
@@ -679,18 +576,12 @@
     <t>aat:300014069</t>
   </si>
   <si>
-    <t>linen (material)</t>
-  </si>
-  <si>
     <t>mahogany</t>
   </si>
   <si>
     <t>aat:300012221</t>
   </si>
   <si>
-    <t>mahogany (wood)</t>
-  </si>
-  <si>
     <t>mahogany panel</t>
   </si>
   <si>
@@ -706,9 +597,6 @@
     <t>aat:300012264</t>
   </si>
   <si>
-    <t>oak (wood)</t>
-  </si>
-  <si>
     <t>oak panel</t>
   </si>
   <si>
@@ -718,96 +606,60 @@
     <t>aat:300014657</t>
   </si>
   <si>
-    <t>panel (wood by form)</t>
-  </si>
-  <si>
     <t>paper</t>
   </si>
   <si>
     <t>aat:300014109</t>
   </si>
   <si>
-    <t>paper (fiber product)</t>
-  </si>
-  <si>
     <t>parchment</t>
   </si>
   <si>
     <t>aat:300011851</t>
   </si>
   <si>
-    <t>parchment (animal material)</t>
-  </si>
-  <si>
     <t>pearwood</t>
   </si>
   <si>
     <t>aat:300012338</t>
   </si>
   <si>
-    <t>pear (wood)</t>
-  </si>
-  <si>
     <t>pine</t>
   </si>
   <si>
     <t>aat:300012620</t>
   </si>
   <si>
-    <t>pine (wood)</t>
-  </si>
-  <si>
-    <t>poplar</t>
-  </si>
-  <si>
     <t>aat:300012363</t>
   </si>
   <si>
-    <t>poplar (wood)</t>
-  </si>
-  <si>
     <t>silk</t>
   </si>
   <si>
     <t>aat:300014072</t>
   </si>
   <si>
-    <t>silk (silkworm material)</t>
-  </si>
-  <si>
     <t>aat:300011029</t>
   </si>
   <si>
-    <t>silver (metal)</t>
-  </si>
-  <si>
     <t>silver fir</t>
   </si>
   <si>
     <t>aat:300343724</t>
   </si>
   <si>
-    <t>silver fir (wood, European silver fir)</t>
-  </si>
-  <si>
     <t>slate</t>
   </si>
   <si>
     <t>aat:300011646</t>
   </si>
   <si>
-    <t>slate (rock)</t>
-  </si>
-  <si>
     <t>spruce</t>
   </si>
   <si>
     <t>aat:300012746</t>
   </si>
   <si>
-    <t>Norway spruce (wood)</t>
-  </si>
-  <si>
     <t>sundeala board</t>
   </si>
   <si>
@@ -823,9 +675,6 @@
     <t>aat:300010669</t>
   </si>
   <si>
-    <t>terracotta (clay material)</t>
-  </si>
-  <si>
     <t>aat:300010678</t>
   </si>
   <si>
@@ -841,9 +690,6 @@
     <t>aat:300133748</t>
   </si>
   <si>
-    <t>tin (metal)</t>
-  </si>
-  <si>
     <t>tracing paper</t>
   </si>
   <si>
@@ -856,18 +702,12 @@
     <t>aat:300011852</t>
   </si>
   <si>
-    <t>vellum (parchment)</t>
-  </si>
-  <si>
     <t>walnut</t>
   </si>
   <si>
     <t>aat:300012476</t>
   </si>
   <si>
-    <t>walnut (wood)</t>
-  </si>
-  <si>
     <t>walnut panel</t>
   </si>
   <si>
@@ -877,27 +717,18 @@
     <t>aat:300011914</t>
   </si>
   <si>
-    <t>wood (plant material)</t>
-  </si>
-  <si>
     <t>wove</t>
   </si>
   <si>
     <t>aat:300014187</t>
   </si>
   <si>
-    <t>wove paper</t>
-  </si>
-  <si>
     <t>yew</t>
   </si>
   <si>
     <t>aat:300012774</t>
   </si>
   <si>
-    <t>yew (wood)</t>
-  </si>
-  <si>
     <t>zinc</t>
   </si>
   <si>
@@ -907,9 +738,6 @@
     <t>aat:300033656</t>
   </si>
   <si>
-    <t>panel paintings (paintings by form)</t>
-  </si>
-  <si>
     <t>aat:300177435</t>
   </si>
   <si>
@@ -919,15 +747,9 @@
     <t>aat:300410350</t>
   </si>
   <si>
-    <t>canvas paintings</t>
-  </si>
-  <si>
     <t>aat:300033936</t>
   </si>
   <si>
-    <t>miniatures (paintings)</t>
-  </si>
-  <si>
     <t>Drying Oil</t>
   </si>
   <si>
@@ -941,6 +763,252 @@
   </si>
   <si>
     <t>Canvas%2C Transferred from Wood</t>
+  </si>
+  <si>
+    <t>chalk@en</t>
+  </si>
+  <si>
+    <t>wax crayons@en</t>
+  </si>
+  <si>
+    <t>gouache (paint)@en</t>
+  </si>
+  <si>
+    <t>bronze (metal)@en</t>
+  </si>
+  <si>
+    <t>charcoal (material)@en</t>
+  </si>
+  <si>
+    <t>distemper@en</t>
+  </si>
+  <si>
+    <t>oil paint (paint)@en</t>
+  </si>
+  <si>
+    <t>egg (material)@en</t>
+  </si>
+  <si>
+    <t>egg tempera@en</t>
+  </si>
+  <si>
+    <t>egg white@en</t>
+  </si>
+  <si>
+    <t>encaustic paint@en</t>
+  </si>
+  <si>
+    <t>plaster@en</t>
+  </si>
+  <si>
+    <t>glue@en</t>
+  </si>
+  <si>
+    <t>size (material)@en</t>
+  </si>
+  <si>
+    <t>gold leaf@en</t>
+  </si>
+  <si>
+    <t>wash (material)@en</t>
+  </si>
+  <si>
+    <t>gum resin@en</t>
+  </si>
+  <si>
+    <t>house paint@en</t>
+  </si>
+  <si>
+    <t>porphyry@en</t>
+  </si>
+  <si>
+    <t>linseed oil@en</t>
+  </si>
+  <si>
+    <t>tile (material)@en</t>
+  </si>
+  <si>
+    <t>pastels (crayons)@en</t>
+  </si>
+  <si>
+    <t>pens (drawing and writing)@en</t>
+  </si>
+  <si>
+    <t>graphite (mineral)@en</t>
+  </si>
+  <si>
+    <t>plaster of Paris@en</t>
+  </si>
+  <si>
+    <t>silver leaf@en</t>
+  </si>
+  <si>
+    <t>tempera@en</t>
+  </si>
+  <si>
+    <t>egg-oil tempera@en</t>
+  </si>
+  <si>
+    <t>walnut oil@en</t>
+  </si>
+  <si>
+    <t>watercolor (paint)@en</t>
+  </si>
+  <si>
+    <t>Carrara marble@en</t>
+  </si>
+  <si>
+    <t>chalk drawings@en</t>
+  </si>
+  <si>
+    <t>drawings (visual works)@en</t>
+  </si>
+  <si>
+    <t>gouaches (paintings)@en</t>
+  </si>
+  <si>
+    <t>sculpture (visual works)@en</t>
+  </si>
+  <si>
+    <t>charcoal drawings@en</t>
+  </si>
+  <si>
+    <t>tempera paintings@en</t>
+  </si>
+  <si>
+    <t>encaustic paintings (visual works)@en</t>
+  </si>
+  <si>
+    <t>frescoes (paintings)@en</t>
+  </si>
+  <si>
+    <t>watercolors (paintings)@en</t>
+  </si>
+  <si>
+    <t>acrylic paintings (visual works)@en</t>
+  </si>
+  <si>
+    <t>oil paintings (visual works)@en</t>
+  </si>
+  <si>
+    <t>mosaics (visual works)@en</t>
+  </si>
+  <si>
+    <t>pen and ink drawings@en</t>
+  </si>
+  <si>
+    <t>pencil drawings@en</t>
+  </si>
+  <si>
+    <t>beech (wood)@en</t>
+  </si>
+  <si>
+    <t>fiberboard@en</t>
+  </si>
+  <si>
+    <t>canvas (textile material)@en</t>
+  </si>
+  <si>
+    <t>cardboard@en</t>
+  </si>
+  <si>
+    <t>copper (metal)@en</t>
+  </si>
+  <si>
+    <t>fir (wood)@en</t>
+  </si>
+  <si>
+    <t>ivory (material)@en</t>
+  </si>
+  <si>
+    <t>laminated paper@en</t>
+  </si>
+  <si>
+    <t>common lime (wood)@en</t>
+  </si>
+  <si>
+    <t>linen (material)@en</t>
+  </si>
+  <si>
+    <t>mahogany (wood)@en</t>
+  </si>
+  <si>
+    <t>millboard@en</t>
+  </si>
+  <si>
+    <t>oak (wood)@en</t>
+  </si>
+  <si>
+    <t>panel (wood by form)@en</t>
+  </si>
+  <si>
+    <t>paper (fiber product)@en</t>
+  </si>
+  <si>
+    <t>parchment (animal material)@en</t>
+  </si>
+  <si>
+    <t>pear (wood)@en</t>
+  </si>
+  <si>
+    <t>pine (wood)@en</t>
+  </si>
+  <si>
+    <t>poplar (wood)@en</t>
+  </si>
+  <si>
+    <t>silk (silkworm material)@en</t>
+  </si>
+  <si>
+    <t>silver (metal)@en</t>
+  </si>
+  <si>
+    <t>silver fir (wood, European silver fir)@en</t>
+  </si>
+  <si>
+    <t>slate (rock)@en</t>
+  </si>
+  <si>
+    <t>Norway spruce (wood)@en</t>
+  </si>
+  <si>
+    <t>terracotta (clay material)@en</t>
+  </si>
+  <si>
+    <t>ceramic tile@en</t>
+  </si>
+  <si>
+    <t>tin (metal)@en</t>
+  </si>
+  <si>
+    <t>tracing paper@en</t>
+  </si>
+  <si>
+    <t>vellum (parchment)@en</t>
+  </si>
+  <si>
+    <t>walnut (wood)@en</t>
+  </si>
+  <si>
+    <t>wood (plant material)@en</t>
+  </si>
+  <si>
+    <t>wove paper@en</t>
+  </si>
+  <si>
+    <t>yew (wood)@en</t>
+  </si>
+  <si>
+    <t>zinc@en</t>
+  </si>
+  <si>
+    <t>panel paintings (paintings by form)@en</t>
+  </si>
+  <si>
+    <t>canvas paintings@en</t>
+  </si>
+  <si>
+    <t>miniatures (paintings)@en</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1042,7 +1110,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1855,15 +1922,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.26953125" style="1"/>
-    <col min="2" max="2" width="16.453125"/>
-    <col min="3" max="3" width="26.81640625"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.6328125" customWidth="1"/>
     <col min="4" max="4" width="14.26953125"/>
     <col min="5" max="5" width="23.453125"/>
     <col min="6" max="6" width="8.54296875"/>
@@ -1887,158 +1954,158 @@
         <v>84</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="25.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:13" ht="38" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>91</v>
-      </c>
       <c r="L3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>97</v>
+        <v>246</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="38" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>297</v>
+        <v>237</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="38" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="38" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>108</v>
+        <v>101</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>253</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E13" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="13" x14ac:dyDescent="0.3">
@@ -2046,35 +2113,35 @@
         <v>35</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>21</v>
+        <v>247</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>35</v>
@@ -2085,161 +2152,161 @@
         <v>38</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>115</v>
+        <v>256</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="25.5" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="38" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>119</v>
+        <v>110</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>257</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>123</v>
+        <v>113</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>258</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="C22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C23" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="38" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="38" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="38" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>135</v>
+        <v>121</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>263</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="63" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>141</v>
+        <v>265</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="26" x14ac:dyDescent="0.3">
@@ -2247,122 +2314,122 @@
         <v>68</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>145</v>
+        <v>128</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>266</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>108</v>
+        <v>101</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>253</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C31" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="C32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>152</v>
+        <v>269</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="C34" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="38" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="C37" t="s">
-        <v>159</v>
+        <v>138</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="25" x14ac:dyDescent="0.25">
@@ -2373,13 +2440,13 @@
         <v>84</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>85</v>
+        <v>242</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2451,18 +2518,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.453125" style="1"/>
     <col min="2" max="2" width="15.54296875"/>
-    <col min="3" max="3" width="26.453125"/>
-    <col min="4" max="4" width="14.453125"/>
-    <col min="5" max="5" width="22.26953125"/>
-    <col min="7" max="1025" width="8.54296875"/>
+    <col min="3" max="3" width="14.453125"/>
+    <col min="4" max="4" width="22.26953125"/>
+    <col min="6" max="1024" width="8.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
@@ -2470,7 +2536,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2480,8 +2546,8 @@
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
+      <c r="C2" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2489,10 +2555,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>164</v>
+        <v>142</v>
+      </c>
+      <c r="C3" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2500,10 +2566,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>166</v>
+        <v>143</v>
+      </c>
+      <c r="C4" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2513,8 +2579,8 @@
       <c r="B5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>50</v>
+      <c r="C5" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2524,8 +2590,8 @@
       <c r="B6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>20</v>
+      <c r="C6" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2533,7 +2599,6 @@
         <v>21</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -2542,8 +2607,8 @@
       <c r="B8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>26</v>
+      <c r="C8" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2553,8 +2618,8 @@
       <c r="B9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>26</v>
+      <c r="C9" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2562,17 +2627,16 @@
         <v>28</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>168</v>
+        <v>144</v>
+      </c>
+      <c r="C11" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2580,10 +2644,10 @@
         <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>170</v>
+        <v>145</v>
+      </c>
+      <c r="C12" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2591,10 +2655,10 @@
         <v>35</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>172</v>
+        <v>146</v>
+      </c>
+      <c r="C13" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2602,10 +2666,10 @@
         <v>36</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>172</v>
+        <v>146</v>
+      </c>
+      <c r="C14" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2613,38 +2677,34 @@
         <v>37</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="12"/>
+      <c r="B16" s="13"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="12"/>
+      <c r="B17" s="13"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B18" s="5"/>
-      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>174</v>
+        <v>147</v>
+      </c>
+      <c r="C19" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2654,8 +2714,8 @@
       <c r="B20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>50</v>
+      <c r="C20" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2663,10 +2723,10 @@
         <v>51</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>176</v>
+        <v>148</v>
+      </c>
+      <c r="C21" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2674,21 +2734,21 @@
         <v>54</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>178</v>
+        <v>150</v>
+      </c>
+      <c r="C22" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>57</v>
+        <v>237</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>176</v>
+        <v>148</v>
+      </c>
+      <c r="C23" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2696,10 +2756,10 @@
         <v>58</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>176</v>
+        <v>148</v>
+      </c>
+      <c r="C24" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2707,10 +2767,10 @@
         <v>59</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>164</v>
+        <v>142</v>
+      </c>
+      <c r="C25" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2720,8 +2780,8 @@
       <c r="B26" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="13" t="s">
-        <v>64</v>
+      <c r="C26" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2731,8 +2791,8 @@
       <c r="B27" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>67</v>
+      <c r="C27" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2742,8 +2802,8 @@
       <c r="B28" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>50</v>
+      <c r="C28" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2751,18 +2811,17 @@
         <v>69</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>170</v>
+        <v>145</v>
+      </c>
+      <c r="C29" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="12"/>
+      <c r="B30" s="13"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -2771,8 +2830,8 @@
       <c r="B31" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>26</v>
+      <c r="C31" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2782,14 +2841,14 @@
       <c r="B32" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="13" t="s">
-        <v>26</v>
+      <c r="C32" t="s">
+        <v>278</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2797,28 +2856,27 @@
         <v>75</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>176</v>
+        <v>148</v>
+      </c>
+      <c r="C33" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="12"/>
+      <c r="B34" s="13"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>172</v>
+        <v>146</v>
+      </c>
+      <c r="C35" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2828,8 +2886,8 @@
       <c r="B36" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>50</v>
+      <c r="C36" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -2839,8 +2897,8 @@
       <c r="B37" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>4</v>
+      <c r="C37" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2869,11 +2927,11 @@
     <hyperlink ref="B29" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
     <hyperlink ref="B31" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
     <hyperlink ref="B32" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
-    <hyperlink ref="D32" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
-    <hyperlink ref="B33" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
-    <hyperlink ref="B35" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
-    <hyperlink ref="B36" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
-    <hyperlink ref="B37" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="B33" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="B35" r:id="rId26" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="B36" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="B37" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="D32" r:id="rId29" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId30"/>
@@ -2886,10 +2944,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2902,565 +2960,580 @@
   <sheetData>
     <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>184</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>156</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C3" t="s">
-        <v>187</v>
+        <v>157</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>301</v>
+        <v>158</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>190</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>241</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>190</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>160</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>192</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>161</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>196</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>187</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>198</v>
+        <v>166</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>187</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>200</v>
+        <v>157</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>201</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>204</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>205</v>
+        <v>170</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>207</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>208</v>
+        <v>172</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>209</v>
+        <v>173</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>210</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>211</v>
+        <v>174</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>210</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>212</v>
+        <v>176</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>213</v>
+        <v>175</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>214</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>215</v>
+        <v>177</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>216</v>
+        <v>178</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>217</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>218</v>
+        <v>179</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>216</v>
+        <v>180</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>217</v>
+        <v>297</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>219</v>
+        <v>181</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>219</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>221</v>
+        <v>182</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>222</v>
+        <v>183</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>223</v>
+        <v>298</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>224</v>
+        <v>184</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>222</v>
+        <v>185</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>223</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>226</v>
+        <v>185</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>227</v>
+        <v>299</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>228</v>
+        <v>187</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>229</v>
+        <v>188</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>230</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>231</v>
+        <v>189</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>232</v>
+        <v>190</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>233</v>
+        <v>301</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>234</v>
+        <v>191</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>235</v>
+        <v>192</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>236</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>237</v>
+        <v>193</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>238</v>
+        <v>194</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>239</v>
+        <v>303</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>195</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>107</v>
+        <v>196</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>108</v>
+        <v>304</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>145</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>298</v>
+        <v>68</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>241</v>
+        <v>128</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>242</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>244</v>
+        <v>197</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>245</v>
+        <v>305</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>198</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>246</v>
+        <v>199</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>247</v>
+        <v>306</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>248</v>
+        <v>72</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>249</v>
+        <v>200</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>250</v>
+        <v>307</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>251</v>
+        <v>201</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>252</v>
+        <v>202</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>253</v>
+        <v>308</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>254</v>
+        <v>203</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>255</v>
+        <v>204</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>256</v>
+        <v>309</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>257</v>
-      </c>
-      <c r="B34" s="5"/>
+        <v>205</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>258</v>
+        <v>207</v>
       </c>
       <c r="B35" s="5"/>
+      <c r="C35" s="4"/>
     </row>
     <row r="36" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>259</v>
+        <v>208</v>
       </c>
       <c r="B36" s="5"/>
+      <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>260</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>264</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>265</v>
+        <v>210</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>263</v>
+        <v>211</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>264</v>
+        <v>311</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>266</v>
+        <v>214</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>267</v>
+        <v>212</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="E39" t="s">
-        <v>196</v>
+        <v>312</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>269</v>
+        <v>215</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>270</v>
+        <v>216</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>269</v>
+        <v>313</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="E40" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>271</v>
+        <v>217</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>272</v>
+        <v>218</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>273</v>
+        <v>314</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>274</v>
+        <v>219</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>275</v>
+        <v>220</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>276</v>
+        <v>315</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>277</v>
+        <v>221</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>275</v>
+        <v>222</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>276</v>
+        <v>316</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>299</v>
+        <v>223</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>279</v>
+        <v>222</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>280</v>
+        <v>316</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>281</v>
+        <v>239</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>282</v>
+        <v>225</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>283</v>
+        <v>317</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>300</v>
+        <v>226</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>285</v>
+        <v>227</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>286</v>
+        <v>318</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>287</v>
+        <v>240</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>288</v>
+        <v>229</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>287</v>
+        <v>319</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>230</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
-    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
-    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
-    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
-    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
-    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
-    <hyperlink ref="B18" r:id="rId17" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
-    <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
-    <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
-    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0300-000013000000}"/>
-    <hyperlink ref="B22" r:id="rId21" xr:uid="{00000000-0004-0000-0300-000014000000}"/>
-    <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0300-000015000000}"/>
-    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0300-000016000000}"/>
-    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0300-000017000000}"/>
-    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0300-000018000000}"/>
-    <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0300-000019000000}"/>
-    <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0300-00001A000000}"/>
-    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0300-00001B000000}"/>
-    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0300-00001C000000}"/>
-    <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0300-00001D000000}"/>
-    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0300-00001E000000}"/>
-    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0300-00001F000000}"/>
-    <hyperlink ref="B37" r:id="rId33" xr:uid="{00000000-0004-0000-0300-000020000000}"/>
-    <hyperlink ref="D37" r:id="rId34" xr:uid="{00000000-0004-0000-0300-000021000000}"/>
-    <hyperlink ref="B38" r:id="rId35" xr:uid="{00000000-0004-0000-0300-000022000000}"/>
-    <hyperlink ref="B39" r:id="rId36" xr:uid="{00000000-0004-0000-0300-000023000000}"/>
-    <hyperlink ref="D39" r:id="rId37" xr:uid="{00000000-0004-0000-0300-000024000000}"/>
-    <hyperlink ref="B40" r:id="rId38" xr:uid="{00000000-0004-0000-0300-000025000000}"/>
-    <hyperlink ref="B41" r:id="rId39" xr:uid="{00000000-0004-0000-0300-000026000000}"/>
-    <hyperlink ref="B42" r:id="rId40" xr:uid="{00000000-0004-0000-0300-000027000000}"/>
-    <hyperlink ref="B43" r:id="rId41" xr:uid="{00000000-0004-0000-0300-000028000000}"/>
-    <hyperlink ref="B44" r:id="rId42" xr:uid="{00000000-0004-0000-0300-000029000000}"/>
-    <hyperlink ref="B45" r:id="rId43" xr:uid="{00000000-0004-0000-0300-00002A000000}"/>
-    <hyperlink ref="B46" r:id="rId44" xr:uid="{00000000-0004-0000-0300-00002B000000}"/>
-    <hyperlink ref="B47" r:id="rId45" xr:uid="{00000000-0004-0000-0300-00002C000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
+    <hyperlink ref="B21" r:id="rId19" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" xr:uid="{00000000-0004-0000-0300-000013000000}"/>
+    <hyperlink ref="B23" r:id="rId21" xr:uid="{00000000-0004-0000-0300-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" xr:uid="{00000000-0004-0000-0300-000015000000}"/>
+    <hyperlink ref="B25" r:id="rId23" xr:uid="{00000000-0004-0000-0300-000016000000}"/>
+    <hyperlink ref="B26" r:id="rId24" xr:uid="{00000000-0004-0000-0300-000017000000}"/>
+    <hyperlink ref="B27" r:id="rId25" xr:uid="{00000000-0004-0000-0300-000018000000}"/>
+    <hyperlink ref="B28" r:id="rId26" xr:uid="{00000000-0004-0000-0300-000019000000}"/>
+    <hyperlink ref="B29" r:id="rId27" xr:uid="{00000000-0004-0000-0300-00001A000000}"/>
+    <hyperlink ref="B30" r:id="rId28" xr:uid="{00000000-0004-0000-0300-00001B000000}"/>
+    <hyperlink ref="B31" r:id="rId29" xr:uid="{00000000-0004-0000-0300-00001C000000}"/>
+    <hyperlink ref="B32" r:id="rId30" xr:uid="{00000000-0004-0000-0300-00001D000000}"/>
+    <hyperlink ref="B33" r:id="rId31" xr:uid="{00000000-0004-0000-0300-00001E000000}"/>
+    <hyperlink ref="B34" r:id="rId32" xr:uid="{00000000-0004-0000-0300-00001F000000}"/>
+    <hyperlink ref="B38" r:id="rId33" xr:uid="{00000000-0004-0000-0300-000020000000}"/>
+    <hyperlink ref="D38" r:id="rId34" xr:uid="{00000000-0004-0000-0300-000021000000}"/>
+    <hyperlink ref="B39" r:id="rId35" xr:uid="{00000000-0004-0000-0300-000022000000}"/>
+    <hyperlink ref="B40" r:id="rId36" xr:uid="{00000000-0004-0000-0300-000023000000}"/>
+    <hyperlink ref="D40" r:id="rId37" xr:uid="{00000000-0004-0000-0300-000024000000}"/>
+    <hyperlink ref="B41" r:id="rId38" xr:uid="{00000000-0004-0000-0300-000025000000}"/>
+    <hyperlink ref="B42" r:id="rId39" xr:uid="{00000000-0004-0000-0300-000026000000}"/>
+    <hyperlink ref="B43" r:id="rId40" xr:uid="{00000000-0004-0000-0300-000027000000}"/>
+    <hyperlink ref="B44" r:id="rId41" xr:uid="{00000000-0004-0000-0300-000028000000}"/>
+    <hyperlink ref="B45" r:id="rId42" xr:uid="{00000000-0004-0000-0300-000029000000}"/>
+    <hyperlink ref="B46" r:id="rId43" xr:uid="{00000000-0004-0000-0300-00002A000000}"/>
+    <hyperlink ref="B47" r:id="rId44" xr:uid="{00000000-0004-0000-0300-00002B000000}"/>
+    <hyperlink ref="B48" r:id="rId45" xr:uid="{00000000-0004-0000-0300-00002C000000}"/>
+    <hyperlink ref="B4" r:id="rId46" xr:uid="{FBD76384-F082-4197-9A59-8D9A173A6834}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3475,7 +3548,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3490,524 +3565,547 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E2" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>156</v>
       </c>
       <c r="B3" s="5"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>241</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>293</v>
+        <v>235</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>294</v>
+        <v>322</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E4" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>160</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>293</v>
+        <v>235</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>294</v>
+        <v>322</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E5" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>161</v>
       </c>
       <c r="B6" s="5"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>163</v>
       </c>
       <c r="B7" s="5"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>166</v>
       </c>
       <c r="B8" s="5"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>198</v>
+        <v>167</v>
       </c>
       <c r="B9" s="5"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>199</v>
+        <v>168</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E10" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>295</v>
-      </c>
-      <c r="C11" t="s">
-        <v>296</v>
+        <v>236</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>205</v>
+        <v>172</v>
       </c>
       <c r="B12" s="5"/>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E13" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>211</v>
+        <v>176</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E14" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>212</v>
+        <v>177</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>293</v>
+        <v>235</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>294</v>
+        <v>322</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E15" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E16" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>218</v>
+        <v>181</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E17" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>219</v>
+        <v>182</v>
       </c>
       <c r="B18" s="5"/>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>221</v>
+        <v>184</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E19" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>224</v>
+        <v>186</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E20" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>225</v>
+        <v>187</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E21" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>228</v>
+        <v>189</v>
       </c>
       <c r="B22" s="5"/>
+      <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>231</v>
+        <v>191</v>
       </c>
       <c r="B23" s="5"/>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>193</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="E24" t="s">
         <v>234</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="E24" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>237</v>
+        <v>195</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E25" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B26" s="5"/>
+      <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>68</v>
       </c>
       <c r="B27" s="5"/>
+      <c r="C27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E28" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>243</v>
+        <v>198</v>
       </c>
       <c r="B29" s="5"/>
+      <c r="C29" s="4"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>72</v>
       </c>
       <c r="B30" s="5"/>
+      <c r="C30" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>248</v>
+        <v>201</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E31" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>251</v>
+        <v>203</v>
       </c>
       <c r="B32" s="5"/>
+      <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>254</v>
+        <v>205</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E33" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>257</v>
+        <v>207</v>
       </c>
       <c r="B34" s="5"/>
+      <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>258</v>
+        <v>208</v>
       </c>
       <c r="B35" s="5"/>
+      <c r="C35" s="4"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>259</v>
+        <v>209</v>
       </c>
       <c r="B36" s="5"/>
+      <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>260</v>
+        <v>210</v>
       </c>
       <c r="B37" s="5"/>
+      <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>265</v>
+        <v>214</v>
       </c>
       <c r="B38" s="5"/>
+      <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>266</v>
+        <v>215</v>
       </c>
       <c r="B39" s="5"/>
+      <c r="C39" s="4"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>269</v>
+        <v>217</v>
       </c>
       <c r="B40" s="5"/>
+      <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>271</v>
+        <v>219</v>
       </c>
       <c r="B41" s="5"/>
+      <c r="C41" s="4"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>274</v>
+        <v>221</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E42" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>277</v>
+        <v>223</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E43" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>278</v>
+        <v>224</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E44" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>281</v>
+        <v>226</v>
       </c>
       <c r="B45" s="5"/>
+      <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>284</v>
+        <v>228</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="E46" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>287</v>
+        <v>230</v>
       </c>
       <c r="B47" s="5"/>
     </row>

</xml_diff>